<commit_message>
its a long night..#done
</commit_message>
<xml_diff>
--- a/src/config/Tax_receipt_form.xlsx
+++ b/src/config/Tax_receipt_form.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OS\Documents\GitHub\Tax-Receipt\src\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Patthawee/Desktop/Tax-Receipt/src/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DB63C8-7E02-5042-9615-220CCCB7AEE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="12160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
   <si>
     <t>รายการ</t>
   </si>
@@ -86,33 +87,12 @@
     <t>วันที่........................................</t>
   </si>
   <si>
-    <t>ภีมรจรัษ  ณควัชรภาณิชภูษิตนิกรโยธิน</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>snack</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>ตึก ECC</t>
-  </si>
-  <si>
-    <t>58010866</t>
-  </si>
-  <si>
-    <t>30.00</t>
-  </si>
-  <si>
-    <t>60.00</t>
-  </si>
-  <si>
-    <t>01/06/2019</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -123,13 +103,89 @@
   </si>
   <si>
     <t>ลงชื่อ..................................ผู้รับของ</t>
+  </si>
+  <si>
+    <t>02/06/2019</t>
+  </si>
+  <si>
+    <t>Patthawee Chumpuvorn</t>
+  </si>
+  <si>
+    <t>พรม</t>
+  </si>
+  <si>
+    <t>200.00</t>
+  </si>
+  <si>
+    <t>หลังคา</t>
+  </si>
+  <si>
+    <t>14.00</t>
+  </si>
+  <si>
+    <t>แผ่นปูพื้น</t>
+  </si>
+  <si>
+    <t>39.00</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>120.00</t>
+  </si>
+  <si>
+    <t>1 prakpak bangsaphannoi prajuabkirikhan</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>78.00</t>
+  </si>
+  <si>
+    <t>42.00</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>480.00</t>
+  </si>
+  <si>
+    <t>neen</t>
+  </si>
+  <si>
+    <t>LnwZa</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>507.00</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>4200.00</t>
+  </si>
+  <si>
+    <t>ทำอะไรก็ได้กูไม่ได้ขอตังใคร้</t>
+  </si>
+  <si>
+    <t>เงินสด</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -375,11 +431,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -393,32 +452,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,28 +786,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37:D37"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" style="6" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="6.83203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="18.83203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="21.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="6" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="10.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="18.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="6.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="9.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="4" width="10.5" collapsed="true"/>
+    <col min="10" max="16384" style="4" width="9.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="18.75">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -763,7 +816,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="18.75">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -772,7 +825,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="18.75">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -781,7 +834,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="18.75">
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -790,7 +843,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="15.75">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -798,20 +851,20 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="20.25">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="15.75">
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -819,12 +872,12 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="20.25">
+    <row r="8" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
@@ -832,18 +885,18 @@
         <v>15</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="20.25">
+    <row r="9" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
@@ -853,26 +906,24 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="20.25">
+    <row r="10" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="C10" s="7"/>
       <c r="D10" s="8"/>
       <c r="E10" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" ht="15.75">
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -880,14 +931,14 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="20.25">
+    <row r="12" spans="1:9" ht="20" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="17" t="s">
         <v>1</v>
       </c>
@@ -901,66 +952,96 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="20.25">
+    <row r="13" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>23</v>
-      </c>
       <c r="D13" s="23" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="20.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+    <row r="14" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>48</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="20.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+    <row r="15" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>46</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="20.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
+    <row r="16" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>48</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="20.25">
+    <row r="17" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="41"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="38"/>
       <c r="D17" s="24"/>
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
@@ -968,10 +1049,10 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" ht="20.25">
+    <row r="18" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="24"/>
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
@@ -979,10 +1060,10 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="20.25">
+    <row r="19" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="24"/>
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
@@ -990,10 +1071,10 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="20.25">
+    <row r="20" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A20" s="18"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="24"/>
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
@@ -1001,10 +1082,10 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="20.25">
+    <row r="21" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="38"/>
       <c r="D21" s="24"/>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
@@ -1012,10 +1093,10 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="20.25">
+    <row r="22" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="24"/>
       <c r="E22" s="21"/>
       <c r="F22" s="21"/>
@@ -1023,10 +1104,10 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="20.25">
+    <row r="23" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="24"/>
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
@@ -1034,10 +1115,10 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" ht="20.25">
+    <row r="24" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A24" s="18"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="24"/>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
@@ -1045,10 +1126,10 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="20.25">
+    <row r="25" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="34"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="24"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
@@ -1056,10 +1137,10 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="20.25">
+    <row r="26" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A26" s="18"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="24"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
@@ -1067,10 +1148,10 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="20.25">
+    <row r="27" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A27" s="18"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="34"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="24"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
@@ -1078,10 +1159,10 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="20.25">
+    <row r="28" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A28" s="18"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="24"/>
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
@@ -1089,10 +1170,10 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" ht="20.25">
+    <row r="29" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="40"/>
       <c r="D29" s="25"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
@@ -1100,51 +1181,53 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="20.25">
+    <row r="30" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A30" s="18"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="32" t="s">
+      <c r="D30" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="32"/>
+      <c r="E30" s="33"/>
       <c r="F30" s="26"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="20.25">
+    <row r="31" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
       <c r="B31" s="13"/>
       <c r="C31" s="14"/>
-      <c r="D31" s="39" t="s">
+      <c r="D31" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="39"/>
+      <c r="E31" s="27"/>
       <c r="F31" s="10"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" ht="20.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="39" t="s">
+    <row r="32" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="39"/>
+      <c r="E32" s="27"/>
       <c r="F32" s="10"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" ht="20.25">
+    <row r="33" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="15"/>
-      <c r="C33" s="7"/>
+      <c r="C33" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="D33" s="8"/>
       <c r="E33" s="14"/>
       <c r="F33" s="8"/>
@@ -1152,7 +1235,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" ht="20.25">
+    <row r="34" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="7"/>
@@ -1163,7 +1246,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" ht="20.25">
+    <row r="35" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="16"/>
@@ -1174,41 +1257,41 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" ht="20.25">
-      <c r="A36" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="37"/>
+    <row r="36" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="A36" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="28"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="20.25">
-      <c r="A37" s="38" t="s">
+    <row r="37" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="A37" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="38"/>
-      <c r="C37" s="38" t="s">
+      <c r="B37" s="29"/>
+      <c r="C37" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38" t="s">
+      <c r="D37" s="29"/>
+      <c r="E37" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F37" s="38"/>
+      <c r="F37" s="29"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" ht="20.25">
+    <row r="38" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1219,7 +1302,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" ht="20.25">
+    <row r="39" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1230,7 +1313,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" ht="20.25">
+    <row r="40" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1241,7 +1324,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" ht="20.25">
+    <row r="41" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1252,7 +1335,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" ht="20.25">
+    <row r="42" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1263,7 +1346,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" ht="20.25">
+    <row r="43" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1274,7 +1357,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" ht="20.25">
+    <row r="44" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1282,7 +1365,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:9" ht="20.25">
+    <row r="45" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1290,7 +1373,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:9" ht="20.25">
+    <row r="46" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1298,7 +1381,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:9" ht="20.25">
+    <row r="47" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1306,7 +1389,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:9" ht="20.25">
+    <row r="48" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1314,7 +1397,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" ht="20.25">
+    <row r="49" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1324,19 +1407,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="B12:C12"/>
@@ -1353,6 +1423,19 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>